<commit_message>
added Policia, OPM and DCR tabs
</commit_message>
<xml_diff>
--- a/data/Departamento_de_correccion_y_rehabilitacion/dcrCasosInv.xlsx
+++ b/data/Departamento_de_correccion_y_rehabilitacion/dcrCasosInv.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariana.pagan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixbaez822/Desktop/ViolenciaGeneroPR/data/Departamento_de_correccion_y_rehabilitacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7BB0D4-7544-3346-B63C-093C59509781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24270" windowHeight="10830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24280" windowHeight="10840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,16 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,9 +39,6 @@
     <t>Femenino</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -65,11 +53,14 @@
   <si>
     <t>year</t>
   </si>
+  <si>
+    <t>Ambos Sexos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,39 +405,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,7 +454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -480,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -497,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -514,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -531,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -548,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -565,7 +556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -582,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -599,7 +590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -616,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -633,7 +624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -650,7 +641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -667,7 +658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -684,7 +675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -701,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -718,7 +709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
@@ -735,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -752,7 +743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -769,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -786,7 +777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -803,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
@@ -820,7 +811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>11</v>
       </c>
@@ -837,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>12</v>
       </c>
@@ -854,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -871,7 +862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -888,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -905,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -922,7 +913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -939,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -956,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -973,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>6</v>
       </c>
@@ -990,7 +981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1007,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1024,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -1041,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10</v>
       </c>
@@ -1058,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>11</v>
       </c>
@@ -1075,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>12</v>
       </c>
@@ -1092,7 +1083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1109,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1126,7 +1117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -1143,7 +1134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1160,7 +1151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1177,7 +1168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>6</v>
       </c>
@@ -1194,7 +1185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>7</v>
       </c>
@@ -1211,7 +1202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>8</v>
       </c>
@@ -1228,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>9</v>
       </c>
@@ -1245,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>10</v>
       </c>
@@ -1262,7 +1253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>11</v>
       </c>
@@ -1279,7 +1270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>12</v>
       </c>
@@ -1296,7 +1287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1313,7 +1304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -1330,7 +1321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1347,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1364,7 +1355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1381,7 +1372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>4</v>
       </c>
@@ -1398,7 +1389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>5</v>
       </c>
@@ -1415,7 +1406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>6</v>
       </c>
@@ -1432,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>7</v>
       </c>
@@ -1449,7 +1440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8</v>
       </c>
@@ -1466,7 +1457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>9</v>
       </c>
@@ -1483,7 +1474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>10</v>
       </c>
@@ -1500,7 +1491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>11</v>
       </c>
@@ -1517,7 +1508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>12</v>
       </c>
@@ -1534,7 +1525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>
@@ -1551,7 +1542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1568,7 +1559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>3</v>
       </c>
@@ -1585,7 +1576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>4</v>
       </c>
@@ -1602,7 +1593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>5</v>
       </c>
@@ -1619,7 +1610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>6</v>
       </c>
@@ -1636,7 +1627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>7</v>
       </c>
@@ -1653,7 +1644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>8</v>
       </c>
@@ -1670,7 +1661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>9</v>
       </c>
@@ -1687,7 +1678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>10</v>
       </c>
@@ -1704,7 +1695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>11</v>
       </c>
@@ -1721,7 +1712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>12</v>
       </c>
@@ -1738,7 +1729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -1755,7 +1746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2</v>
       </c>
@@ -1772,7 +1763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -1789,7 +1780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2</v>
       </c>
@@ -1806,7 +1797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>3</v>
       </c>
@@ -1823,7 +1814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>4</v>
       </c>
@@ -1840,7 +1831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>5</v>
       </c>
@@ -1857,7 +1848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>6</v>
       </c>
@@ -1874,7 +1865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>7</v>
       </c>
@@ -1891,7 +1882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>8</v>
       </c>
@@ -1908,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>9</v>
       </c>
@@ -1925,7 +1916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>10</v>
       </c>
@@ -1942,7 +1933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>11</v>
       </c>
@@ -1959,7 +1950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>12</v>
       </c>
@@ -1976,7 +1967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -1993,7 +1984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2</v>
       </c>
@@ -2010,7 +2001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>3</v>
       </c>
@@ -2027,7 +2018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>4</v>
       </c>
@@ -2044,7 +2035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>5</v>
       </c>
@@ -2061,7 +2052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>6</v>
       </c>
@@ -2078,7 +2069,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>7</v>
       </c>
@@ -2095,7 +2086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>8</v>
       </c>
@@ -2112,7 +2103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>9</v>
       </c>
@@ -2129,7 +2120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>10</v>
       </c>
@@ -2146,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>11</v>
       </c>
@@ -2163,7 +2154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>12</v>
       </c>
@@ -2180,7 +2171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1</v>
       </c>
@@ -2197,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2</v>
       </c>
@@ -2214,7 +2205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1</v>
       </c>
@@ -2228,10 +2219,10 @@
         <v>66</v>
       </c>
       <c r="E106" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2</v>
       </c>
@@ -2245,10 +2236,10 @@
         <v>96</v>
       </c>
       <c r="E107" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>3</v>
       </c>
@@ -2262,10 +2253,10 @@
         <v>104</v>
       </c>
       <c r="E108" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>4</v>
       </c>
@@ -2279,10 +2270,10 @@
         <v>110</v>
       </c>
       <c r="E109" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>5</v>
       </c>
@@ -2296,10 +2287,10 @@
         <v>98</v>
       </c>
       <c r="E110" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>6</v>
       </c>
@@ -2313,10 +2304,10 @@
         <v>96</v>
       </c>
       <c r="E111" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>7</v>
       </c>
@@ -2330,10 +2321,10 @@
         <v>113</v>
       </c>
       <c r="E112" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>8</v>
       </c>
@@ -2347,10 +2338,10 @@
         <v>164</v>
       </c>
       <c r="E113" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>9</v>
       </c>
@@ -2364,10 +2355,10 @@
         <v>148</v>
       </c>
       <c r="E114" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>10</v>
       </c>
@@ -2381,10 +2372,10 @@
         <v>153</v>
       </c>
       <c r="E115" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>11</v>
       </c>
@@ -2398,10 +2389,10 @@
         <v>147</v>
       </c>
       <c r="E116" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>12</v>
       </c>
@@ -2415,10 +2406,10 @@
         <v>143</v>
       </c>
       <c r="E117" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>1</v>
       </c>
@@ -2432,10 +2423,10 @@
         <v>124</v>
       </c>
       <c r="E118" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2</v>
       </c>
@@ -2449,10 +2440,10 @@
         <v>134</v>
       </c>
       <c r="E119" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>3</v>
       </c>
@@ -2466,10 +2457,10 @@
         <v>117</v>
       </c>
       <c r="E120" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>4</v>
       </c>
@@ -2483,10 +2474,10 @@
         <v>19</v>
       </c>
       <c r="E121" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>5</v>
       </c>
@@ -2500,10 +2491,10 @@
         <v>110</v>
       </c>
       <c r="E122" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>6</v>
       </c>
@@ -2517,10 +2508,10 @@
         <v>124</v>
       </c>
       <c r="E123" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>7</v>
       </c>
@@ -2534,10 +2525,10 @@
         <v>96</v>
       </c>
       <c r="E124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>8</v>
       </c>
@@ -2551,10 +2542,10 @@
         <v>87</v>
       </c>
       <c r="E125" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>9</v>
       </c>
@@ -2568,10 +2559,10 @@
         <v>6</v>
       </c>
       <c r="E126" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>10</v>
       </c>
@@ -2585,10 +2576,10 @@
         <v>10</v>
       </c>
       <c r="E127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>11</v>
       </c>
@@ -2602,10 +2593,10 @@
         <v>10</v>
       </c>
       <c r="E128" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>12</v>
       </c>
@@ -2619,10 +2610,10 @@
         <v>16</v>
       </c>
       <c r="E129" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1</v>
       </c>
@@ -2636,10 +2627,10 @@
         <v>221</v>
       </c>
       <c r="E130" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2</v>
       </c>
@@ -2653,10 +2644,10 @@
         <v>231</v>
       </c>
       <c r="E131" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1</v>
       </c>
@@ -2670,10 +2661,10 @@
         <v>950</v>
       </c>
       <c r="E132" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2</v>
       </c>
@@ -2687,10 +2678,10 @@
         <v>957</v>
       </c>
       <c r="E133" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>3</v>
       </c>
@@ -2704,10 +2695,10 @@
         <v>1002</v>
       </c>
       <c r="E134" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>4</v>
       </c>
@@ -2721,10 +2712,10 @@
         <v>1016</v>
       </c>
       <c r="E135" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>5</v>
       </c>
@@ -2738,10 +2729,10 @@
         <v>1083</v>
       </c>
       <c r="E136" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>6</v>
       </c>
@@ -2755,10 +2746,10 @@
         <v>998</v>
       </c>
       <c r="E137" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>7</v>
       </c>
@@ -2772,10 +2763,10 @@
         <v>1015</v>
       </c>
       <c r="E138" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>8</v>
       </c>
@@ -2789,10 +2780,10 @@
         <v>1059</v>
       </c>
       <c r="E139" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>9</v>
       </c>
@@ -2806,10 +2797,10 @@
         <v>959</v>
       </c>
       <c r="E140" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>10</v>
       </c>
@@ -2823,10 +2814,10 @@
         <v>1025</v>
       </c>
       <c r="E141" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>11</v>
       </c>
@@ -2840,10 +2831,10 @@
         <v>1063</v>
       </c>
       <c r="E142" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>12</v>
       </c>
@@ -2857,10 +2848,10 @@
         <v>1131</v>
       </c>
       <c r="E143" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1</v>
       </c>
@@ -2874,10 +2865,10 @@
         <v>1234</v>
       </c>
       <c r="E144" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2</v>
       </c>
@@ -2891,10 +2882,10 @@
         <v>1238</v>
       </c>
       <c r="E145" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>3</v>
       </c>
@@ -2908,10 +2899,10 @@
         <v>1312</v>
       </c>
       <c r="E146" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>4</v>
       </c>
@@ -2925,10 +2916,10 @@
         <v>1321</v>
       </c>
       <c r="E147" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>5</v>
       </c>
@@ -2942,10 +2933,10 @@
         <v>1366</v>
       </c>
       <c r="E148" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>6</v>
       </c>
@@ -2959,10 +2950,10 @@
         <v>1182</v>
       </c>
       <c r="E149" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>7</v>
       </c>
@@ -2976,10 +2967,10 @@
         <v>1205</v>
       </c>
       <c r="E150" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>8</v>
       </c>
@@ -2993,10 +2984,10 @@
         <v>1240</v>
       </c>
       <c r="E151" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>9</v>
       </c>
@@ -3010,10 +3001,10 @@
         <v>1098</v>
       </c>
       <c r="E152" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>10</v>
       </c>
@@ -3027,10 +3018,10 @@
         <v>1172</v>
       </c>
       <c r="E153" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>11</v>
       </c>
@@ -3044,10 +3035,10 @@
         <v>1107</v>
       </c>
       <c r="E154" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>12</v>
       </c>
@@ -3061,10 +3052,10 @@
         <v>1164</v>
       </c>
       <c r="E155" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>1</v>
       </c>
@@ -3078,10 +3069,10 @@
         <v>1507</v>
       </c>
       <c r="E156" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2</v>
       </c>
@@ -3095,7 +3086,7 @@
         <v>1561</v>
       </c>
       <c r="E157" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new data for Dept. Correccion y Rehabilitacion
</commit_message>
<xml_diff>
--- a/data/Departamento_de_correccion_y_rehabilitacion/dcrCasosInv.xlsx
+++ b/data/Departamento_de_correccion_y_rehabilitacion/dcrCasosInv.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="10">
   <si>
     <t>Investigaciones  realizadas</t>
   </si>
@@ -406,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E217"/>
+  <dimension ref="A1:E223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="1">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>2</v>
@@ -1470,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>2</v>
@@ -1487,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="1">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>2</v>
@@ -1665,41 +1665,41 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B74" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" s="1">
-        <v>2</v>
+        <v>1333</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B75" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75" s="1">
-        <v>3</v>
+        <v>1196</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B76" s="1">
         <v>2021</v>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="D76" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>3</v>
@@ -1716,7 +1716,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="1">
         <v>2021</v>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="D77" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>3</v>
@@ -1733,7 +1733,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B78" s="1">
         <v>2021</v>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="D78" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>3</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B79" s="1">
         <v>2021</v>
@@ -1759,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="D79" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>3</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B80" s="1">
         <v>2021</v>
@@ -1776,7 +1776,7 @@
         <v>0</v>
       </c>
       <c r="D80" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>3</v>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1">
         <v>2021</v>
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="D81" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>3</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B82" s="1">
         <v>2021</v>
@@ -1810,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="D82" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>3</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B83" s="1">
         <v>2021</v>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="D83" s="1">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>3</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B84" s="1">
         <v>2021</v>
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="D84" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>3</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B85" s="1">
         <v>2021</v>
@@ -1861,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="D85" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>3</v>
@@ -1869,16 +1869,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B86" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D86" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>3</v>
@@ -1886,16 +1886,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B87" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D87" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>3</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B88" s="1">
         <v>2022</v>
@@ -1912,7 +1912,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>3</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B89" s="1">
         <v>2022</v>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B90" s="1">
         <v>2022</v>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="D90" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>3</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
+        <v>4</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1">
         <v>6</v>
-      </c>
-      <c r="B91" s="1">
-        <v>2022</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D91" s="1">
-        <v>8</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>3</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B92" s="1">
         <v>2022</v>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="D92" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>3</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B93" s="1">
         <v>2022</v>
@@ -2005,7 +2005,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B94" s="1">
         <v>2022</v>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="D94" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>3</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B95" s="1">
         <v>2022</v>
@@ -2031,7 +2031,7 @@
         <v>0</v>
       </c>
       <c r="D95" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>3</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B96" s="1">
         <v>2022</v>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="D96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>3</v>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B97" s="1">
         <v>2022</v>
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="D97" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>3</v>
@@ -2073,16 +2073,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B98" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D98" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>3</v>
@@ -2090,16 +2090,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B99" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D99" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>3</v>
@@ -2110,13 +2110,13 @@
         <v>1</v>
       </c>
       <c r="B100" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" s="1">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>3</v>
@@ -2127,13 +2127,13 @@
         <v>2</v>
       </c>
       <c r="B101" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="1">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>3</v>
@@ -2141,7 +2141,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B102" s="1">
         <v>2021</v>
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="1">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>3</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B103" s="1">
         <v>2021</v>
@@ -2167,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="D103" s="1">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>3</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B104" s="1">
         <v>2021</v>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
       <c r="D104" s="1">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>3</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B105" s="1">
         <v>2021</v>
@@ -2201,7 +2201,7 @@
         <v>1</v>
       </c>
       <c r="D105" s="1">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>3</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B106" s="1">
         <v>2021</v>
@@ -2218,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="D106" s="1">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>3</v>
@@ -2226,7 +2226,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B107" s="1">
         <v>2021</v>
@@ -2235,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="D107" s="1">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>3</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B108" s="1">
         <v>2021</v>
@@ -2252,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="D108" s="1">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>3</v>
@@ -2260,7 +2260,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B109" s="1">
         <v>2021</v>
@@ -2269,7 +2269,7 @@
         <v>1</v>
       </c>
       <c r="D109" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>3</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B110" s="1">
         <v>2021</v>
@@ -2286,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="D110" s="1">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>3</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B111" s="1">
         <v>2021</v>
@@ -2303,7 +2303,7 @@
         <v>1</v>
       </c>
       <c r="D111" s="1">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>3</v>
@@ -2311,16 +2311,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B112" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D112" s="1">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>3</v>
@@ -2328,16 +2328,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B113" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D113" s="1">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>3</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B114" s="1">
         <v>2022</v>
@@ -2354,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="D114" s="1">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>3</v>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B115" s="1">
         <v>2022</v>
@@ -2371,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="D115" s="1">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>3</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B116" s="1">
         <v>2022</v>
@@ -2388,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="D116" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>3</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B117" s="1">
         <v>2022</v>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="D117" s="1">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>3</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B118" s="1">
         <v>2022</v>
@@ -2422,7 +2422,7 @@
         <v>1</v>
       </c>
       <c r="D118" s="1">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>3</v>
@@ -2430,7 +2430,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B119" s="1">
         <v>2022</v>
@@ -2439,7 +2439,7 @@
         <v>1</v>
       </c>
       <c r="D119" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>3</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B120" s="1">
         <v>2022</v>
@@ -2464,7 +2464,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B121" s="1">
         <v>2022</v>
@@ -2473,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="D121" s="1">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>3</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B122" s="1">
         <v>2022</v>
@@ -2490,7 +2490,7 @@
         <v>1</v>
       </c>
       <c r="D122" s="1">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>3</v>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B123" s="1">
         <v>2022</v>
@@ -2507,7 +2507,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="1">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>3</v>
@@ -2515,16 +2515,16 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B124" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D124" s="1">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>3</v>
@@ -2532,16 +2532,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B125" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D125" s="1">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>3</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B126" s="1">
         <v>2023</v>
@@ -2558,7 +2558,7 @@
         <v>1</v>
       </c>
       <c r="D126" s="1">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>3</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B127" s="1">
         <v>2023</v>
@@ -2575,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="D127" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>3</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B128" s="1">
         <v>2023</v>
@@ -2592,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="D128" s="1">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>3</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B129" s="1">
         <v>2023</v>
@@ -2609,7 +2609,7 @@
         <v>1</v>
       </c>
       <c r="D129" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>3</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B130" s="1">
         <v>2023</v>
@@ -2626,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="D130" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>3</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B131" s="1">
         <v>2023</v>
@@ -2643,7 +2643,7 @@
         <v>1</v>
       </c>
       <c r="D131" s="1">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>3</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B132" s="1">
         <v>2023</v>
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="D132" s="1">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>3</v>
@@ -2668,7 +2668,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B133" s="1">
         <v>2023</v>
@@ -2677,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="D133" s="1">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>3</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B134" s="1">
         <v>2023</v>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="D134" s="1">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>3</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B135" s="1">
         <v>2023</v>
@@ -2711,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="D135" s="1">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>3</v>
@@ -2719,16 +2719,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B136" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D136" s="1">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>3</v>
@@ -2736,16 +2736,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B137" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D137" s="1">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>3</v>
@@ -2753,7 +2753,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B138" s="1">
         <v>2024</v>
@@ -2762,7 +2762,7 @@
         <v>1</v>
       </c>
       <c r="D138" s="1">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>3</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B139" s="1">
         <v>2024</v>
@@ -2779,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="D139" s="1">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>3</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B140" s="1">
         <v>2024</v>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="D140" s="1">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>3</v>
@@ -2804,7 +2804,7 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B141" s="1">
         <v>2024</v>
@@ -2813,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="D141" s="1">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>3</v>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B142" s="1">
         <v>2024</v>
@@ -2830,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="D142" s="1">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>3</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B143" s="1">
         <v>2024</v>
@@ -2847,7 +2847,7 @@
         <v>1</v>
       </c>
       <c r="D143" s="1">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>3</v>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B144" s="1">
         <v>2024</v>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="D144" s="1">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>3</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B145" s="1">
         <v>2024</v>
@@ -2881,7 +2881,7 @@
         <v>1</v>
       </c>
       <c r="D145" s="1">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>3</v>
@@ -2889,75 +2889,75 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B146" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D146" s="1">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B147" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D147" s="1">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B148" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D148" s="1">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B149" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B150" s="1">
         <v>2021</v>
@@ -2966,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="D150" s="1">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>9</v>
@@ -2974,7 +2974,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B151" s="1">
         <v>2021</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B152" s="1">
         <v>2021</v>
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="D152" s="1">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>9</v>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B153" s="1">
         <v>2021</v>
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="D153" s="1">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>9</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B154" s="1">
         <v>2021</v>
@@ -3034,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="D154" s="1">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>9</v>
@@ -3042,7 +3042,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B155" s="1">
         <v>2021</v>
@@ -3051,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="D155" s="1">
-        <v>153</v>
+        <v>96</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>9</v>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B156" s="1">
         <v>2021</v>
@@ -3068,7 +3068,7 @@
         <v>0</v>
       </c>
       <c r="D156" s="1">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>9</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B157" s="1">
         <v>2021</v>
@@ -3085,7 +3085,7 @@
         <v>0</v>
       </c>
       <c r="D157" s="1">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>9</v>
@@ -3093,16 +3093,16 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B158" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D158" s="1">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>9</v>
@@ -3110,16 +3110,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B159" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D159" s="1">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>9</v>
@@ -3127,16 +3127,16 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B160" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D160" s="1">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>9</v>
@@ -3144,16 +3144,16 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B161" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D161" s="1">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>9</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B162" s="1">
         <v>2022</v>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="D162" s="1">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>9</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B163" s="1">
         <v>2022</v>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="D163" s="1">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>9</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B164" s="1">
         <v>2022</v>
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="D164" s="1">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>9</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B165" s="1">
         <v>2022</v>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="D165" s="1">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>9</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B166" s="1">
         <v>2022</v>
@@ -3238,7 +3238,7 @@
         <v>0</v>
       </c>
       <c r="D166" s="1">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>9</v>
@@ -3246,7 +3246,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B167" s="1">
         <v>2022</v>
@@ -3255,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="D167" s="1">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>9</v>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B168" s="1">
         <v>2022</v>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="D168" s="1">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>9</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B169" s="1">
         <v>2022</v>
@@ -3289,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="D169" s="1">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>9</v>
@@ -3297,16 +3297,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B170" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D170" s="1">
-        <v>221</v>
+        <v>6</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>9</v>
@@ -3314,16 +3314,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B171" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D171" s="1">
-        <v>231</v>
+        <v>10</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>9</v>
@@ -3331,16 +3331,16 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B172" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D172" s="1">
-        <v>950</v>
+        <v>10</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>9</v>
@@ -3348,16 +3348,16 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B173" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D173" s="1">
-        <v>957</v>
+        <v>16</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>9</v>
@@ -3365,16 +3365,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B174" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D174" s="1">
-        <v>1002</v>
+        <v>221</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>9</v>
@@ -3382,16 +3382,16 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B175" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D175" s="1">
-        <v>1016</v>
+        <v>231</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>9</v>
@@ -3399,7 +3399,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B176" s="1">
         <v>2021</v>
@@ -3408,7 +3408,7 @@
         <v>1</v>
       </c>
       <c r="D176" s="1">
-        <v>1083</v>
+        <v>950</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>9</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B177" s="1">
         <v>2021</v>
@@ -3425,7 +3425,7 @@
         <v>1</v>
       </c>
       <c r="D177" s="1">
-        <v>998</v>
+        <v>957</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>9</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B178" s="1">
         <v>2021</v>
@@ -3442,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="D178" s="1">
-        <v>1015</v>
+        <v>1002</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>9</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B179" s="1">
         <v>2021</v>
@@ -3459,7 +3459,7 @@
         <v>1</v>
       </c>
       <c r="D179" s="1">
-        <v>1059</v>
+        <v>1016</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>9</v>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B180" s="1">
         <v>2021</v>
@@ -3476,7 +3476,7 @@
         <v>1</v>
       </c>
       <c r="D180" s="1">
-        <v>959</v>
+        <v>1083</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>9</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B181" s="1">
         <v>2021</v>
@@ -3493,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="D181" s="1">
-        <v>1025</v>
+        <v>998</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>9</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B182" s="1">
         <v>2021</v>
@@ -3510,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="D182" s="1">
-        <v>1063</v>
+        <v>1015</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>9</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B183" s="1">
         <v>2021</v>
@@ -3527,7 +3527,7 @@
         <v>1</v>
       </c>
       <c r="D183" s="1">
-        <v>1131</v>
+        <v>1059</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>9</v>
@@ -3535,16 +3535,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B184" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D184" s="1">
-        <v>1234</v>
+        <v>959</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>9</v>
@@ -3552,16 +3552,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B185" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D185" s="1">
-        <v>1238</v>
+        <v>1025</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>9</v>
@@ -3569,16 +3569,16 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B186" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D186" s="1">
-        <v>1312</v>
+        <v>1063</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>9</v>
@@ -3586,16 +3586,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B187" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D187" s="1">
-        <v>1321</v>
+        <v>1131</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>9</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B188" s="1">
         <v>2022</v>
@@ -3612,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="D188" s="1">
-        <v>1366</v>
+        <v>1234</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>9</v>
@@ -3620,7 +3620,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B189" s="1">
         <v>2022</v>
@@ -3629,7 +3629,7 @@
         <v>1</v>
       </c>
       <c r="D189" s="1">
-        <v>1182</v>
+        <v>1238</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>9</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B190" s="1">
         <v>2022</v>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="D190" s="1">
-        <v>1205</v>
+        <v>1312</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>9</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B191" s="1">
         <v>2022</v>
@@ -3663,7 +3663,7 @@
         <v>1</v>
       </c>
       <c r="D191" s="1">
-        <v>1240</v>
+        <v>1321</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>9</v>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B192" s="1">
         <v>2022</v>
@@ -3680,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="D192" s="1">
-        <v>1098</v>
+        <v>1366</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>9</v>
@@ -3688,7 +3688,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B193" s="1">
         <v>2022</v>
@@ -3697,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="D193" s="1">
-        <v>1172</v>
+        <v>1182</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>9</v>
@@ -3705,7 +3705,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B194" s="1">
         <v>2022</v>
@@ -3714,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="D194" s="1">
-        <v>1107</v>
+        <v>1205</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>9</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B195" s="1">
         <v>2022</v>
@@ -3731,7 +3731,7 @@
         <v>1</v>
       </c>
       <c r="D195" s="1">
-        <v>1164</v>
+        <v>1240</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>9</v>
@@ -3739,16 +3739,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B196" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D196" s="1">
-        <v>1507</v>
+        <v>1098</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>9</v>
@@ -3756,16 +3756,16 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B197" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D197" s="1">
-        <v>1561</v>
+        <v>1172</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>9</v>
@@ -3773,16 +3773,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B198" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D198" s="1">
-        <v>1552</v>
+        <v>1107</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>9</v>
@@ -3790,16 +3790,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B199" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D199" s="1">
-        <v>1519</v>
+        <v>1164</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>9</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B200" s="1">
         <v>2023</v>
@@ -3816,7 +3816,7 @@
         <v>1</v>
       </c>
       <c r="D200" s="1">
-        <v>1498</v>
+        <v>1507</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>9</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B201" s="1">
         <v>2023</v>
@@ -3833,7 +3833,7 @@
         <v>1</v>
       </c>
       <c r="D201" s="1">
-        <v>1512</v>
+        <v>1561</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>9</v>
@@ -3841,7 +3841,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B202" s="1">
         <v>2023</v>
@@ -3850,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="D202" s="1">
-        <v>1512</v>
+        <v>1552</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>9</v>
@@ -3858,7 +3858,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B203" s="1">
         <v>2023</v>
@@ -3867,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="D203" s="1">
-        <v>1490</v>
+        <v>1519</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>9</v>
@@ -3875,7 +3875,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B204" s="1">
         <v>2023</v>
@@ -3884,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="D204" s="1">
-        <v>1497</v>
+        <v>1498</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>9</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B205" s="1">
         <v>2023</v>
@@ -3901,7 +3901,7 @@
         <v>1</v>
       </c>
       <c r="D205" s="1">
-        <v>1431</v>
+        <v>1512</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>9</v>
@@ -3909,7 +3909,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B206" s="1">
         <v>2023</v>
@@ -3918,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="D206" s="1">
-        <v>1463</v>
+        <v>1512</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>9</v>
@@ -3926,7 +3926,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B207" s="1">
         <v>2023</v>
@@ -3935,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="D207" s="1">
-        <v>1388</v>
+        <v>1490</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>9</v>
@@ -3943,16 +3943,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B208" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D208" s="1">
-        <v>1385</v>
+        <v>1497</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>9</v>
@@ -3960,16 +3960,16 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B209" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D209" s="1">
-        <v>1426</v>
+        <v>1430</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>9</v>
@@ -3977,16 +3977,16 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B210" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D210" s="1">
-        <v>1420</v>
+        <v>1462</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>9</v>
@@ -3994,16 +3994,16 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B211" s="1">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D211" s="1">
-        <v>1456</v>
+        <v>1387</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>9</v>
@@ -4011,7 +4011,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B212" s="1">
         <v>2024</v>
@@ -4020,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="D212" s="1">
-        <v>1368</v>
+        <v>1385</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>9</v>
@@ -4028,7 +4028,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B213" s="1">
         <v>2024</v>
@@ -4037,7 +4037,7 @@
         <v>1</v>
       </c>
       <c r="D213" s="1">
-        <v>1322</v>
+        <v>1426</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>9</v>
@@ -4045,7 +4045,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B214" s="1">
         <v>2024</v>
@@ -4054,7 +4054,7 @@
         <v>1</v>
       </c>
       <c r="D214" s="1">
-        <v>1489</v>
+        <v>1420</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>9</v>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B215" s="1">
         <v>2024</v>
@@ -4071,7 +4071,7 @@
         <v>1</v>
       </c>
       <c r="D215" s="1">
-        <v>1359</v>
+        <v>1456</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>9</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B216" s="1">
         <v>2024</v>
@@ -4088,7 +4088,7 @@
         <v>1</v>
       </c>
       <c r="D216" s="1">
-        <v>1558</v>
+        <v>1368</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>9</v>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B217" s="1">
         <v>2024</v>
@@ -4105,9 +4105,111 @@
         <v>1</v>
       </c>
       <c r="D217" s="1">
+        <v>1322</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>7</v>
+      </c>
+      <c r="B218" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D218" s="1">
+        <v>1489</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>8</v>
+      </c>
+      <c r="B219" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D219" s="1">
+        <v>1359</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>9</v>
+      </c>
+      <c r="B220" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D220" s="1">
+        <v>1558</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>10</v>
+      </c>
+      <c r="B221" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D221" s="1">
         <v>1580</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="E221" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>11</v>
+      </c>
+      <c r="B222" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D222" s="1">
+        <v>1452</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>12</v>
+      </c>
+      <c r="B223" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D223" s="1">
+        <v>1305</v>
+      </c>
+      <c r="E223" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify data in Dept. Correccion
</commit_message>
<xml_diff>
--- a/data/Departamento_de_correccion_y_rehabilitacion/dcrCasosInv.xlsx
+++ b/data/Departamento_de_correccion_y_rehabilitacion/dcrCasosInv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Departamento_de_correccion_y_rehabilitacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFCA972-4C61-4337-93D8-61CF17F54C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B7F315-4B1B-4440-A544-408AE4AAB9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31680" yWindow="1905" windowWidth="24885" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -421,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G350" sqref="G350"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2279,7 +2277,7 @@
       <c r="C109" t="s">
         <v>1</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109">
         <v>1323</v>
       </c>
       <c r="E109" t="s">
@@ -2296,7 +2294,7 @@
       <c r="C110" t="s">
         <v>1</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110">
         <v>1394</v>
       </c>
       <c r="E110" t="s">
@@ -2313,7 +2311,7 @@
       <c r="C111" t="s">
         <v>1</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111">
         <v>1543</v>
       </c>
       <c r="E111" t="s">
@@ -2330,7 +2328,7 @@
       <c r="C112" t="s">
         <v>1</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112">
         <v>1551</v>
       </c>
       <c r="E112" t="s">
@@ -2347,7 +2345,7 @@
       <c r="C113" t="s">
         <v>1</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113">
         <v>1571</v>
       </c>
       <c r="E113" t="s">
@@ -2364,7 +2362,7 @@
       <c r="C114" t="s">
         <v>1</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114">
         <v>1538</v>
       </c>
       <c r="E114" t="s">
@@ -2381,7 +2379,7 @@
       <c r="C115" t="s">
         <v>1</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115">
         <v>1482</v>
       </c>
       <c r="E115" t="s">
@@ -2398,7 +2396,7 @@
       <c r="C116" t="s">
         <v>1</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116">
         <v>1551</v>
       </c>
       <c r="E116" t="s">
@@ -2415,7 +2413,7 @@
       <c r="C117" t="s">
         <v>1</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117">
         <v>1551</v>
       </c>
       <c r="E117" t="s">
@@ -2432,7 +2430,7 @@
       <c r="C118" t="s">
         <v>1</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118">
         <v>1419</v>
       </c>
       <c r="E118" t="s">
@@ -2449,7 +2447,7 @@
       <c r="C119" t="s">
         <v>1</v>
       </c>
-      <c r="D119" s="1">
+      <c r="D119">
         <v>1510</v>
       </c>
       <c r="E119" t="s">
@@ -2466,7 +2464,7 @@
       <c r="C120" t="s">
         <v>1</v>
       </c>
-      <c r="D120" s="1">
+      <c r="D120">
         <v>1410</v>
       </c>
       <c r="E120" t="s">
@@ -2483,7 +2481,7 @@
       <c r="C121" t="s">
         <v>1</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D121">
         <v>1561</v>
       </c>
       <c r="E121" t="s">
@@ -3306,207 +3304,207 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="1">
-        <v>1</v>
-      </c>
-      <c r="B170" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C170" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D170" s="1">
-        <v>0</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="1">
-        <v>2</v>
-      </c>
-      <c r="B171" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D171" s="1">
-        <v>0</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="1">
-        <v>3</v>
-      </c>
-      <c r="B172" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D172" s="1">
-        <v>0</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="1">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>1</v>
+      </c>
+      <c r="B170">
+        <v>2025</v>
+      </c>
+      <c r="C170" t="s">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>2</v>
+      </c>
+      <c r="B171">
+        <v>2025</v>
+      </c>
+      <c r="C171" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>3</v>
+      </c>
+      <c r="B172">
+        <v>2025</v>
+      </c>
+      <c r="C172" t="s">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173">
         <v>4</v>
       </c>
-      <c r="B173" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C173" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D173" s="1">
-        <v>0</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="1">
+      <c r="B173">
+        <v>2025</v>
+      </c>
+      <c r="C173" t="s">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174">
         <v>5</v>
       </c>
-      <c r="B174" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D174" s="1">
-        <v>0</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="1">
+      <c r="B174">
+        <v>2025</v>
+      </c>
+      <c r="C174" t="s">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175">
         <v>6</v>
       </c>
-      <c r="B175" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D175" s="1">
-        <v>0</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="1">
+      <c r="B175">
+        <v>2025</v>
+      </c>
+      <c r="C175" t="s">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176">
         <v>7</v>
       </c>
-      <c r="B176" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D176" s="1">
-        <v>0</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="1">
+      <c r="B176">
+        <v>2025</v>
+      </c>
+      <c r="C176" t="s">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177">
         <v>8</v>
       </c>
-      <c r="B177" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D177" s="1">
-        <v>0</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="1">
-        <v>9</v>
-      </c>
-      <c r="B178" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D178" s="1">
-        <v>0</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="1">
+      <c r="B177">
+        <v>2025</v>
+      </c>
+      <c r="C177" t="s">
+        <v>0</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>9</v>
+      </c>
+      <c r="B178">
+        <v>2025</v>
+      </c>
+      <c r="C178" t="s">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179">
         <v>10</v>
       </c>
-      <c r="B179" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D179" s="1">
-        <v>0</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="1">
+      <c r="B179">
+        <v>2025</v>
+      </c>
+      <c r="C179" t="s">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180">
         <v>11</v>
       </c>
-      <c r="B180" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D180" s="1">
-        <v>0</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="1">
+      <c r="B180">
+        <v>2025</v>
+      </c>
+      <c r="C180" t="s">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181">
         <v>12</v>
       </c>
-      <c r="B181" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D181" s="1">
-        <v>0</v>
-      </c>
-      <c r="E181" s="1" t="s">
+      <c r="B181">
+        <v>2025</v>
+      </c>
+      <c r="C181" t="s">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4319,214 +4317,214 @@
       <c r="C229" t="s">
         <v>1</v>
       </c>
-      <c r="D229" s="2">
+      <c r="D229">
         <v>119</v>
       </c>
       <c r="E229" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="230" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="1">
-        <v>1</v>
-      </c>
-      <c r="B230" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D230" s="2">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>1</v>
+      </c>
+      <c r="B230">
+        <v>2025</v>
+      </c>
+      <c r="C230" t="s">
+        <v>1</v>
+      </c>
+      <c r="D230">
         <v>123</v>
       </c>
-      <c r="E230" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="1">
-        <v>2</v>
-      </c>
-      <c r="B231" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D231" s="2">
+      <c r="E230" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>2</v>
+      </c>
+      <c r="B231">
+        <v>2025</v>
+      </c>
+      <c r="C231" t="s">
+        <v>1</v>
+      </c>
+      <c r="D231">
         <v>139</v>
       </c>
-      <c r="E231" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="1">
-        <v>3</v>
-      </c>
-      <c r="B232" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D232" s="2">
+      <c r="E231" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>3</v>
+      </c>
+      <c r="B232">
+        <v>2025</v>
+      </c>
+      <c r="C232" t="s">
+        <v>1</v>
+      </c>
+      <c r="D232">
         <v>131</v>
       </c>
-      <c r="E232" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="1">
+      <c r="E232" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A233">
         <v>4</v>
       </c>
-      <c r="B233" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D233" s="2">
+      <c r="B233">
+        <v>2025</v>
+      </c>
+      <c r="C233" t="s">
+        <v>1</v>
+      </c>
+      <c r="D233">
         <v>132</v>
       </c>
-      <c r="E233" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="1">
+      <c r="E233" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A234">
         <v>5</v>
       </c>
-      <c r="B234" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D234" s="2">
+      <c r="B234">
+        <v>2025</v>
+      </c>
+      <c r="C234" t="s">
+        <v>1</v>
+      </c>
+      <c r="D234">
         <v>135</v>
       </c>
-      <c r="E234" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="1">
+      <c r="E234" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A235">
         <v>6</v>
       </c>
-      <c r="B235" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D235" s="2">
+      <c r="B235">
+        <v>2025</v>
+      </c>
+      <c r="C235" t="s">
+        <v>1</v>
+      </c>
+      <c r="D235">
         <v>131</v>
       </c>
-      <c r="E235" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="1">
+      <c r="E235" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A236">
         <v>7</v>
       </c>
-      <c r="B236" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D236" s="2">
+      <c r="B236">
+        <v>2025</v>
+      </c>
+      <c r="C236" t="s">
+        <v>1</v>
+      </c>
+      <c r="D236">
         <v>136</v>
       </c>
-      <c r="E236" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="1">
+      <c r="E236" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A237">
         <v>8</v>
       </c>
-      <c r="B237" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D237" s="2">
+      <c r="B237">
+        <v>2025</v>
+      </c>
+      <c r="C237" t="s">
+        <v>1</v>
+      </c>
+      <c r="D237">
         <v>133</v>
       </c>
-      <c r="E237" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="1">
-        <v>9</v>
-      </c>
-      <c r="B238" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D238" s="2">
+      <c r="E237" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>9</v>
+      </c>
+      <c r="B238">
+        <v>2025</v>
+      </c>
+      <c r="C238" t="s">
+        <v>1</v>
+      </c>
+      <c r="D238">
         <v>126</v>
       </c>
-      <c r="E238" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="1">
+      <c r="E238" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A239">
         <v>10</v>
       </c>
-      <c r="B239" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D239" s="2">
+      <c r="B239">
+        <v>2025</v>
+      </c>
+      <c r="C239" t="s">
+        <v>1</v>
+      </c>
+      <c r="D239">
         <v>141</v>
       </c>
-      <c r="E239" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="1">
+      <c r="E239" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A240">
         <v>11</v>
       </c>
-      <c r="B240" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D240" s="2">
+      <c r="B240">
+        <v>2025</v>
+      </c>
+      <c r="C240" t="s">
+        <v>1</v>
+      </c>
+      <c r="D240">
         <v>137</v>
       </c>
-      <c r="E240" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="1">
+      <c r="E240" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A241">
         <v>12</v>
       </c>
-      <c r="B241" s="1">
-        <v>2025</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D241" s="2">
+      <c r="B241">
+        <v>2025</v>
+      </c>
+      <c r="C241" t="s">
+        <v>1</v>
+      </c>
+      <c r="D241">
         <v>151</v>
       </c>
-      <c r="E241" s="1" t="s">
+      <c r="E241" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5346,207 +5344,207 @@
         <v>9</v>
       </c>
     </row>
-    <row r="290" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A290" s="2">
-        <v>1</v>
-      </c>
-      <c r="B290" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D290" s="2">
-        <v>0</v>
-      </c>
-      <c r="E290" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="291" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A291" s="2">
-        <v>2</v>
-      </c>
-      <c r="B291" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C291" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D291" s="2">
-        <v>0</v>
-      </c>
-      <c r="E291" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="292" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="2">
-        <v>3</v>
-      </c>
-      <c r="B292" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D292" s="2">
-        <v>0</v>
-      </c>
-      <c r="E292" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="293" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A293" s="2">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>1</v>
+      </c>
+      <c r="B290">
+        <v>2025</v>
+      </c>
+      <c r="C290" t="s">
+        <v>0</v>
+      </c>
+      <c r="D290">
+        <v>0</v>
+      </c>
+      <c r="E290" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>2</v>
+      </c>
+      <c r="B291">
+        <v>2025</v>
+      </c>
+      <c r="C291" t="s">
+        <v>0</v>
+      </c>
+      <c r="D291">
+        <v>0</v>
+      </c>
+      <c r="E291" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>3</v>
+      </c>
+      <c r="B292">
+        <v>2025</v>
+      </c>
+      <c r="C292" t="s">
+        <v>0</v>
+      </c>
+      <c r="D292">
+        <v>0</v>
+      </c>
+      <c r="E292" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A293">
         <v>4</v>
       </c>
-      <c r="B293" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D293" s="2">
-        <v>0</v>
-      </c>
-      <c r="E293" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="294" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A294" s="2">
+      <c r="B293">
+        <v>2025</v>
+      </c>
+      <c r="C293" t="s">
+        <v>0</v>
+      </c>
+      <c r="D293">
+        <v>0</v>
+      </c>
+      <c r="E293" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A294">
         <v>5</v>
       </c>
-      <c r="B294" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D294" s="2">
-        <v>0</v>
-      </c>
-      <c r="E294" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="295" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="2">
+      <c r="B294">
+        <v>2025</v>
+      </c>
+      <c r="C294" t="s">
+        <v>0</v>
+      </c>
+      <c r="D294">
+        <v>0</v>
+      </c>
+      <c r="E294" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A295">
         <v>6</v>
       </c>
-      <c r="B295" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D295" s="2">
-        <v>0</v>
-      </c>
-      <c r="E295" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="296" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A296" s="2">
+      <c r="B295">
+        <v>2025</v>
+      </c>
+      <c r="C295" t="s">
+        <v>0</v>
+      </c>
+      <c r="D295">
+        <v>0</v>
+      </c>
+      <c r="E295" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A296">
         <v>7</v>
       </c>
-      <c r="B296" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C296" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D296" s="2">
-        <v>0</v>
-      </c>
-      <c r="E296" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="297" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A297" s="2">
+      <c r="B296">
+        <v>2025</v>
+      </c>
+      <c r="C296" t="s">
+        <v>0</v>
+      </c>
+      <c r="D296">
+        <v>0</v>
+      </c>
+      <c r="E296" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A297">
         <v>8</v>
       </c>
-      <c r="B297" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D297" s="2">
-        <v>0</v>
-      </c>
-      <c r="E297" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="298" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A298" s="2">
-        <v>9</v>
-      </c>
-      <c r="B298" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C298" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D298" s="2">
-        <v>0</v>
-      </c>
-      <c r="E298" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="299" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A299" s="2">
+      <c r="B297">
+        <v>2025</v>
+      </c>
+      <c r="C297" t="s">
+        <v>0</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>9</v>
+      </c>
+      <c r="B298">
+        <v>2025</v>
+      </c>
+      <c r="C298" t="s">
+        <v>0</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A299">
         <v>10</v>
       </c>
-      <c r="B299" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C299" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D299" s="2">
-        <v>0</v>
-      </c>
-      <c r="E299" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="300" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A300" s="2">
+      <c r="B299">
+        <v>2025</v>
+      </c>
+      <c r="C299" t="s">
+        <v>0</v>
+      </c>
+      <c r="D299">
+        <v>0</v>
+      </c>
+      <c r="E299" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A300">
         <v>11</v>
       </c>
-      <c r="B300" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C300" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D300" s="2">
-        <v>0</v>
-      </c>
-      <c r="E300" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="301" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A301" s="2">
+      <c r="B300">
+        <v>2025</v>
+      </c>
+      <c r="C300" t="s">
+        <v>0</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A301">
         <v>12</v>
       </c>
-      <c r="B301" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C301" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D301" s="2">
-        <v>0</v>
-      </c>
-      <c r="E301" s="2" t="s">
+      <c r="B301">
+        <v>2025</v>
+      </c>
+      <c r="C301" t="s">
+        <v>0</v>
+      </c>
+      <c r="D301">
+        <v>0</v>
+      </c>
+      <c r="E301" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6367,206 +6365,206 @@
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A350" s="2">
-        <v>1</v>
-      </c>
-      <c r="B350" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C350" s="2" t="s">
+      <c r="A350">
+        <v>1</v>
+      </c>
+      <c r="B350">
+        <v>2025</v>
+      </c>
+      <c r="C350" t="s">
         <v>1</v>
       </c>
       <c r="D350">
         <v>1517</v>
       </c>
-      <c r="E350" s="2" t="s">
+      <c r="E350" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A351" s="2">
-        <v>2</v>
-      </c>
-      <c r="B351" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C351" s="2" t="s">
+      <c r="A351">
+        <v>2</v>
+      </c>
+      <c r="B351">
+        <v>2025</v>
+      </c>
+      <c r="C351" t="s">
         <v>1</v>
       </c>
       <c r="D351">
         <v>1682</v>
       </c>
-      <c r="E351" s="2" t="s">
+      <c r="E351" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A352" s="2">
-        <v>3</v>
-      </c>
-      <c r="B352" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C352" s="2" t="s">
+      <c r="A352">
+        <v>3</v>
+      </c>
+      <c r="B352">
+        <v>2025</v>
+      </c>
+      <c r="C352" t="s">
         <v>1</v>
       </c>
       <c r="D352">
         <v>1682</v>
       </c>
-      <c r="E352" s="2" t="s">
+      <c r="E352" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A353" s="2">
+      <c r="A353">
         <v>4</v>
       </c>
-      <c r="B353" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C353" s="2" t="s">
+      <c r="B353">
+        <v>2025</v>
+      </c>
+      <c r="C353" t="s">
         <v>1</v>
       </c>
       <c r="D353">
         <v>1703</v>
       </c>
-      <c r="E353" s="2" t="s">
+      <c r="E353" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A354" s="2">
+      <c r="A354">
         <v>5</v>
       </c>
-      <c r="B354" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C354" s="2" t="s">
+      <c r="B354">
+        <v>2025</v>
+      </c>
+      <c r="C354" t="s">
         <v>1</v>
       </c>
       <c r="D354">
         <v>1673</v>
       </c>
-      <c r="E354" s="2" t="s">
+      <c r="E354" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A355" s="2">
+      <c r="A355">
         <v>6</v>
       </c>
-      <c r="B355" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C355" s="2" t="s">
+      <c r="B355">
+        <v>2025</v>
+      </c>
+      <c r="C355" t="s">
         <v>1</v>
       </c>
       <c r="D355">
         <v>1613</v>
       </c>
-      <c r="E355" s="2" t="s">
+      <c r="E355" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A356" s="2">
+      <c r="A356">
         <v>7</v>
       </c>
-      <c r="B356" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C356" s="2" t="s">
+      <c r="B356">
+        <v>2025</v>
+      </c>
+      <c r="C356" t="s">
         <v>1</v>
       </c>
       <c r="D356">
         <v>1687</v>
       </c>
-      <c r="E356" s="2" t="s">
+      <c r="E356" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A357" s="2">
+      <c r="A357">
         <v>8</v>
       </c>
-      <c r="B357" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C357" s="2" t="s">
+      <c r="B357">
+        <v>2025</v>
+      </c>
+      <c r="C357" t="s">
         <v>1</v>
       </c>
       <c r="D357">
         <v>1684</v>
       </c>
-      <c r="E357" s="2" t="s">
+      <c r="E357" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A358" s="2">
-        <v>9</v>
-      </c>
-      <c r="B358" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C358" s="2" t="s">
+      <c r="A358">
+        <v>9</v>
+      </c>
+      <c r="B358">
+        <v>2025</v>
+      </c>
+      <c r="C358" t="s">
         <v>1</v>
       </c>
       <c r="D358">
         <v>1545</v>
       </c>
-      <c r="E358" s="2" t="s">
+      <c r="E358" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A359" s="2">
+      <c r="A359">
         <v>10</v>
       </c>
-      <c r="B359" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C359" s="2" t="s">
+      <c r="B359">
+        <v>2025</v>
+      </c>
+      <c r="C359" t="s">
         <v>1</v>
       </c>
       <c r="D359">
         <v>1651</v>
       </c>
-      <c r="E359" s="2" t="s">
+      <c r="E359" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A360" s="2">
+      <c r="A360">
         <v>11</v>
       </c>
-      <c r="B360" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C360" s="2" t="s">
+      <c r="B360">
+        <v>2025</v>
+      </c>
+      <c r="C360" t="s">
         <v>1</v>
       </c>
       <c r="D360">
         <v>1547</v>
       </c>
-      <c r="E360" s="2" t="s">
+      <c r="E360" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A361" s="2">
+      <c r="A361">
         <v>12</v>
       </c>
-      <c r="B361" s="2">
-        <v>2025</v>
-      </c>
-      <c r="C361" s="2" t="s">
+      <c r="B361">
+        <v>2025</v>
+      </c>
+      <c r="C361" t="s">
         <v>1</v>
       </c>
       <c r="D361">
         <v>1712</v>
       </c>
-      <c r="E361" s="2" t="s">
+      <c r="E361" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>